<commit_message>
edited test_file1 is commited
</commit_message>
<xml_diff>
--- a/Test_Data/Credkart_Test_Data.xlsx
+++ b/Test_Data/Credkart_Test_Data.xlsx
@@ -478,12 +478,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>login_fail</t>
+          <t>login_pass</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
     </row>

</xml_diff>